<commit_message>
also doing nr topics 20 reg fitting
</commit_message>
<xml_diff>
--- a/full_workflow_analysis.xlsx
+++ b/full_workflow_analysis.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/cd5619e07473d5e8/Dokumente/winfoMaster/Masterarbeit/bertopic_ecc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="6" documentId="8_{4C0686E9-A492-456A-8259-5543585FA475}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{647B8717-7C63-49A8-9948-9C6E8214A72B}"/>
+  <xr:revisionPtr revIDLastSave="11" documentId="8_{4C0686E9-A492-456A-8259-5543585FA475}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1897B505-467A-4BD5-B5CF-CDE08FFFA94E}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{7F1F1C6D-2529-49DA-A5D3-69E34F68FC10}"/>
+    <workbookView xWindow="4830" yWindow="1890" windowWidth="21630" windowHeight="11310" xr2:uid="{7F1F1C6D-2529-49DA-A5D3-69E34F68FC10}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="25">
   <si>
     <t>topic quality</t>
   </si>
@@ -108,6 +108,9 @@
   </si>
   <si>
     <t>zeroshot</t>
+  </si>
+  <si>
+    <t>.-&gt; 6700 nachdem etwas toleranz für die industry calls eingebaut wurde!S9</t>
   </si>
 </sst>
 </file>
@@ -479,15 +482,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A8A7A47-BF54-4F93-AEC4-8C6F2E3312CC}">
-  <dimension ref="B2:W5"/>
+  <dimension ref="B2:W6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R12" sqref="R12"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="2" spans="2:23" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:23" x14ac:dyDescent="0.25">
       <c r="I2" t="s">
         <v>12</v>
       </c>
@@ -495,7 +498,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="2:23" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>5</v>
       </c>
@@ -539,7 +542,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="2:23" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B4">
         <v>2500</v>
       </c>
@@ -579,8 +582,11 @@
       <c r="R4" t="s">
         <v>18</v>
       </c>
+      <c r="S4" t="s">
+        <v>24</v>
+      </c>
     </row>
-    <row r="5" spans="2:23" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B5">
         <v>2500</v>
       </c>
@@ -592,6 +598,20 @@
       </c>
       <c r="H5" t="s">
         <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B6">
+        <v>2500</v>
+      </c>
+      <c r="C6">
+        <v>300</v>
+      </c>
+      <c r="D6" t="s">
+        <v>3</v>
+      </c>
+      <c r="E6">
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>